<commit_message>
EDA+new us source monthly
</commit_message>
<xml_diff>
--- a/data_source/us-Annual-Arrivals-2000-to-Present–Country-of-Residence.xlsx
+++ b/data_source/us-Annual-Arrivals-2000-to-Present–Country-of-Residence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TERP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karuntarat\Documents\1st Year, 2nd Term\DADs5001\dads-5001-mini-project\data_source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0D8B71-DC54-467D-8E77-F88B181E3E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906069CB-FAAF-4A83-B798-6DBD9E796775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{309E4658-369E-48A8-ACFA-BF02D17567DA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{309E4658-369E-48A8-ACFA-BF02D17567DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Annual" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="311">
   <si>
     <r>
       <rPr>
@@ -1010,6 +1010,12 @@
   <si>
     <t>World Region</t>
   </si>
+  <si>
+    <t>Countries</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
 </sst>
 </file>
 
@@ -1121,7 +1127,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1171,6 +1177,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1192,7 +1202,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="CIC Monthly Data Layout"/>
@@ -2380,7 +2390,7 @@
       <selection activeCell="Z29" sqref="Z29"/>
       <selection pane="topRight" activeCell="Z29" sqref="Z29"/>
       <selection pane="bottomLeft" activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -2395,9 +2405,9 @@
     <col min="28" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="44.4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:27" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>309</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>308</v>
@@ -2467,6 +2477,9 @@
       </c>
       <c r="Y1" s="3">
         <v>2021</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="AA1" s="4" t="s">
         <v>1</v>

</xml_diff>